<commit_message>
Commit and push in to the github
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19380" windowHeight="6495" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15210" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:T20"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
@@ -383,7 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>